<commit_message>
built demo for cash flow parser
</commit_message>
<xml_diff>
--- a/data/input_dataset_v.1.xlsx
+++ b/data/input_dataset_v.1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="96">
   <si>
     <t xml:space="preserve">Transaction_ID</t>
   </si>
@@ -40,9 +40,6 @@
     <t xml:space="preserve">Amount_EUR</t>
   </si>
   <si>
-    <t xml:space="preserve">IDEAL_RESULT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Invoice #45-A, Agricultural diesel</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t xml:space="preserve">1,200.00</t>
   </si>
   <si>
-    <t xml:space="preserve">Agricultural diesel</t>
-  </si>
-  <si>
     <t xml:space="preserve">Electricity Bill - Offices</t>
   </si>
   <si>
@@ -70,9 +64,6 @@
     <t xml:space="preserve">350.00</t>
   </si>
   <si>
-    <t xml:space="preserve">Electricity Bill</t>
-  </si>
-  <si>
     <t xml:space="preserve">Payment for legal services</t>
   </si>
   <si>
@@ -85,7 +76,7 @@
     <t xml:space="preserve">2,500.00</t>
   </si>
   <si>
-    <t xml:space="preserve">Purchase Ammonium Nitrate 10tons</t>
+    <t xml:space="preserve">Purchase Ammonium Nitrate 10,000tons</t>
   </si>
   <si>
     <t xml:space="preserve">Fertilizers Co.</t>
@@ -94,18 +85,12 @@
     <t xml:space="preserve">7,000.00</t>
   </si>
   <si>
-    <t xml:space="preserve">Ammonium Nitrate</t>
-  </si>
-  <si>
     <t xml:space="preserve">Electricity Bill - Irrigation Pumps</t>
   </si>
   <si>
     <t xml:space="preserve">1,800.00</t>
   </si>
   <si>
-    <t xml:space="preserve">Electricity Bill </t>
-  </si>
-  <si>
     <t xml:space="preserve">Tractor T-100 Maintenance</t>
   </si>
   <si>
@@ -124,9 +109,6 @@
     <t xml:space="preserve">1,500.00</t>
   </si>
   <si>
-    <t xml:space="preserve">Diesel fuel</t>
-  </si>
-  <si>
     <t xml:space="preserve">Office stationery purchase</t>
   </si>
   <si>
@@ -145,18 +127,12 @@
     <t xml:space="preserve">AgriChem Solutions</t>
   </si>
   <si>
-    <t xml:space="preserve">Herbicide</t>
-  </si>
-  <si>
     <t xml:space="preserve">Water Bill - Irrigation System</t>
   </si>
   <si>
     <t xml:space="preserve">Municipal Water Authority</t>
   </si>
   <si>
-    <t xml:space="preserve">Water Bill </t>
-  </si>
-  <si>
     <t xml:space="preserve">Annual Insurance Premium</t>
   </si>
   <si>
@@ -172,15 +148,9 @@
     <t xml:space="preserve">Premium Seeds Ltd.</t>
   </si>
   <si>
-    <t xml:space="preserve">Corn Hybrid</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fuel Invoice #102-C</t>
   </si>
   <si>
-    <t xml:space="preserve">Fuel </t>
-  </si>
-  <si>
     <t xml:space="preserve">Harvester Repair - Hydraulic System</t>
   </si>
   <si>
@@ -191,9 +161,6 @@
   </si>
   <si>
     <t xml:space="preserve">Fertilizer - Potassium 8tonne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potassium </t>
   </si>
   <si>
     <t xml:space="preserve">Office Electricity Bill</t>
@@ -630,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G:G"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -641,7 +608,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.57"/>
   </cols>
   <sheetData>
@@ -664,9 +631,6 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -676,19 +640,16 @@
         <v>45672</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -699,19 +660,16 @@
         <v>45677</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,18 +680,15 @@
         <v>45679</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -745,20 +700,18 @@
         <v>45685</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -768,20 +721,18 @@
         <v>45690</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -791,19 +742,16 @@
         <v>45698</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -814,19 +762,16 @@
         <v>45703</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -837,19 +782,16 @@
         <v>45708</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -860,20 +802,18 @@
         <v>45721</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>3200</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -883,20 +823,18 @@
         <v>45724</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>890</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -906,19 +844,16 @@
         <v>45728</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>4500</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -929,19 +864,16 @@
         <v>45734</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" s="1" t="n">
         <v>8500</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -952,19 +884,16 @@
         <v>45738</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>1350</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,19 +904,16 @@
         <v>45744</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>2100</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -998,19 +924,16 @@
         <v>45750</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F16" s="1" t="n">
         <v>1800</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,19 +944,16 @@
         <v>45757</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>5600</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1044,19 +964,16 @@
         <v>45762</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>425</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1067,19 +984,16 @@
         <v>45767</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F19" s="1" t="n">
         <v>1250</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,19 +1004,16 @@
         <v>45772</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>680</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,19 +1024,16 @@
         <v>45779</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F21" s="1" t="n">
         <v>950</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,19 +1044,16 @@
         <v>45785</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F22" s="1" t="n">
         <v>1680</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1159,19 +1064,16 @@
         <v>45789</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>340</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,19 +1084,16 @@
         <v>45795</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F24" s="1" t="n">
         <v>1450</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1205,19 +1104,16 @@
         <v>45802</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" s="1" t="n">
         <v>2300</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1228,13 +1124,13 @@
         <v>45811</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" s="1" t="n">
         <v>8400</v>
@@ -1248,13 +1144,13 @@
         <v>45816</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F27" s="1" t="n">
         <v>1250</v>
@@ -1268,13 +1164,13 @@
         <v>45822</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F28" s="1" t="n">
         <v>875</v>
@@ -1288,13 +1184,13 @@
         <v>45827</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F29" s="1" t="n">
         <v>1950</v>
@@ -1308,13 +1204,13 @@
         <v>45832</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F30" s="1" t="n">
         <v>1200</v>
@@ -1328,13 +1224,13 @@
         <v>45838</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F31" s="1" t="n">
         <v>780</v>
@@ -1348,13 +1244,13 @@
         <v>45843</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" s="1" t="n">
         <v>2650</v>
@@ -1368,13 +1264,13 @@
         <v>45849</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F33" s="1" t="n">
         <v>1150</v>
@@ -1388,13 +1284,13 @@
         <v>45854</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F34" s="1" t="n">
         <v>950</v>
@@ -1408,13 +1304,13 @@
         <v>45860</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F35" s="1" t="n">
         <v>2100</v>
@@ -1428,13 +1324,13 @@
         <v>45866</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F36" s="1" t="n">
         <v>1680</v>
@@ -1448,13 +1344,13 @@
         <v>45871</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F37" s="1" t="n">
         <v>540</v>
@@ -1468,13 +1364,13 @@
         <v>45878</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" s="1" t="n">
         <v>2800</v>
@@ -1488,13 +1384,13 @@
         <v>45883</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F39" s="1" t="n">
         <v>2150</v>
@@ -1508,13 +1404,13 @@
         <v>45889</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F40" s="1" t="n">
         <v>3200</v>
@@ -1528,13 +1424,13 @@
         <v>45895</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F41" s="1" t="n">
         <v>1850</v>
@@ -1548,13 +1444,13 @@
         <v>45903</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F42" s="1" t="n">
         <v>1775</v>
@@ -1568,13 +1464,13 @@
         <v>45910</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F43" s="1" t="n">
         <v>4500</v>
@@ -1588,13 +1484,13 @@
         <v>45915</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F44" s="1" t="n">
         <v>3850</v>
@@ -1608,13 +1504,13 @@
         <v>45922</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F45" s="1" t="n">
         <v>5200</v>
@@ -1628,13 +1524,13 @@
         <v>45928</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F46" s="1" t="n">
         <v>980</v>
@@ -1648,13 +1544,13 @@
         <v>45935</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" s="1" t="n">
         <v>4200</v>
@@ -1668,13 +1564,13 @@
         <v>45941</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F48" s="1" t="n">
         <v>1350</v>
@@ -1688,13 +1584,13 @@
         <v>45947</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F49" s="1" t="n">
         <v>3800</v>
@@ -1708,13 +1604,13 @@
         <v>45953</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F50" s="1" t="n">
         <v>2250</v>

</xml_diff>